<commit_message>
shows order details on edit order page
</commit_message>
<xml_diff>
--- a/data/wine_inventory_bad.xlsx
+++ b/data/wine_inventory_bad.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -46,16 +46,50 @@
   </si>
   <si>
     <t>2009 Pinot Noir</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Sparkling</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,13 +112,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -414,15 +464,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A10:F12"/>
+  <dimension ref="A10:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -439,10 +489,16 @@
         <v>4</v>
       </c>
       <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>1</v>
       </c>
@@ -458,11 +514,17 @@
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11">
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>2</v>
       </c>
@@ -475,12 +537,19 @@
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12">
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>